<commit_message>
02_Product_Backlog.xlsx: Product_Backlog auf den aktuellen Stand aktualisiert.
</commit_message>
<xml_diff>
--- a/1. Projektplanung/02_Product_Backlog.xlsx
+++ b/1. Projektplanung/02_Product_Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thude0-my.sharepoint.com/personal/jecklu01_hs-ulm_de/Documents/5. Semester/Software Projekt/RaytRazor/1. Projektplanung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="528" documentId="11_AD4DB114E441178AC67DF4622615E776693EDF11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B795728F-BC4A-48BD-9B5C-A6F89CBD471A}"/>
+  <xr:revisionPtr revIDLastSave="623" documentId="11_AD4DB114E441178AC67DF4622615E776693EDF11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C77E213-AFCB-4715-AAE8-A82D07928517}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
   <si>
     <t>ID</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Grundstruktur des Projekt Repositories auf GitHub anlegen.</t>
   </si>
   <si>
-    <t>Grundstruktur des Raytracers aufsetzen.</t>
-  </si>
-  <si>
     <t>Programmnamen definieren und entsprechendes Logo erstellen.</t>
   </si>
   <si>
@@ -139,6 +136,45 @@
   </si>
   <si>
     <t>Mathematische Formelsammlung bzgl. Raytracing erstellen.</t>
+  </si>
+  <si>
+    <t>Quellennachweis 2.2 (ChatGPT)</t>
+  </si>
+  <si>
+    <t>Gewählt: Java/JavaFX</t>
+  </si>
+  <si>
+    <t>3D-Objekte Interface/Abstract Class definieren.</t>
+  </si>
+  <si>
+    <t>3D-Objekte importierten ermöglichen.</t>
+  </si>
+  <si>
+    <t>Lichtquellen als 3D Objekt deklarieren.</t>
+  </si>
+  <si>
+    <t>Lichtquellen Farbe anpassbar machen.</t>
+  </si>
+  <si>
+    <t>Environment/Skybox aufbauen.</t>
+  </si>
+  <si>
+    <t>Demo Szenen aufbauen.</t>
+  </si>
+  <si>
+    <t>Bild Speicherbar machen.</t>
+  </si>
+  <si>
+    <t>Kamera muss frei bewegbar.</t>
+  </si>
+  <si>
+    <t>Raybounds/Reflektionsanzahl definieren.</t>
+  </si>
+  <si>
+    <t>Benutzeroberfläche des Programms erstellen.</t>
+  </si>
+  <si>
+    <t>3D-Objekt Importer erstellen.</t>
   </si>
 </sst>
 </file>
@@ -326,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -337,34 +373,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -376,56 +409,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -514,7 +505,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -522,40 +512,15 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thick">
-          <color auto="1"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
         </left>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
+        <right/>
         <top/>
         <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -581,7 +546,15 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -635,6 +608,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -642,16 +616,41 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thick">
+          <color auto="1"/>
         </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+        <top style="thick">
+          <color auto="1"/>
+        </top>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -661,13 +660,38 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thick">
           <color auto="1"/>
         </left>
-        <top style="thick">
+        <right style="thick">
           <color auto="1"/>
-        </top>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -690,23 +714,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{637C7F0C-036B-4704-9330-87E77AC2CA73}" name="Tabelle5" displayName="Tabelle5" ref="A3:F16" totalsRowShown="0" headerRowDxfId="4" dataDxfId="5" headerRowBorderDxfId="8" tableBorderDxfId="9">
-  <autoFilter ref="A3:F16" xr:uid="{637C7F0C-036B-4704-9330-87E77AC2CA73}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{637C7F0C-036B-4704-9330-87E77AC2CA73}" name="Tabelle5" displayName="Tabelle5" ref="A3:F26" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
+  <autoFilter ref="A3:F26" xr:uid="{637C7F0C-036B-4704-9330-87E77AC2CA73}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{201166DE-250E-4841-A2FB-745D597FF3E9}" name="Status" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{201166DE-250E-4841-A2FB-745D597FF3E9}" name="Status" dataDxfId="5">
       <calculatedColumnFormula>IF($G$3="", "[Auswählen]")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{A81DA036-E59B-45ED-99C0-7DA578D2F41E}" name="ID" dataDxfId="7">
+    <tableColumn id="2" xr3:uid="{A81DA036-E59B-45ED-99C0-7DA578D2F41E}" name="ID" dataDxfId="4">
       <calculatedColumnFormula>ROW()-ROW('Product Backlog'!$B$3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{67C87643-0AEC-4F3F-93A3-8AEBECB97CD3}" name="Beschreibung" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{39A480AF-C7AB-4A2D-A3A9-017A9988CD1E}" name="Priorität" dataDxfId="6">
+    <tableColumn id="3" xr3:uid="{67C87643-0AEC-4F3F-93A3-8AEBECB97CD3}" name="Beschreibung" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{39A480AF-C7AB-4A2D-A3A9-017A9988CD1E}" name="Priorität" dataDxfId="2">
       <calculatedColumnFormula>IF($G$3="", "[Auswählen]")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F7F4B23B-3880-466E-A27E-72BD382F2D29}" name="Aufwand" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{F7F4B23B-3880-466E-A27E-72BD382F2D29}" name="Aufwand" dataDxfId="1">
       <calculatedColumnFormula>IF($G$3="", "[Auswählen]")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9BFAA39F-E911-47E7-A57A-71690B5E810B}" name="Bemerkung" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{9BFAA39F-E911-47E7-A57A-71690B5E810B}" name="Bemerkung" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -988,10 +1012,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="190" zoomScaleNormal="205" zoomScalePageLayoutView="190" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,58 +1025,58 @@
     <col min="3" max="3" width="52.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" style="18" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="12" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="13"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>1</v>
+      <c r="A4" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="B4" s="4">
         <f>ROW()-ROW('Product Backlog'!$B$3)</f>
@@ -1067,20 +1091,20 @@
       <c r="E4" s="4">
         <v>2</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>1</v>
+      <c r="A5" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="B5" s="4">
         <f>ROW()-ROW('Product Backlog'!$B$3)</f>
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="4">
         <v>5</v>
@@ -1088,20 +1112,20 @@
       <c r="E5" s="4">
         <v>1</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>1</v>
+      <c r="A6" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="B6" s="4">
         <f>ROW()-ROW('Product Backlog'!$B$3)</f>
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="4">
         <v>3</v>
@@ -1109,18 +1133,20 @@
       <c r="E6" s="4">
         <v>2</v>
       </c>
-      <c r="F6" s="17"/>
+      <c r="F6" s="11" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="6">
+      <c r="A7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4">
         <f>ROW()-ROW('Product Backlog'!$B$3)</f>
         <v>4</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="4">
         <v>3</v>
@@ -1128,13 +1154,15 @@
       <c r="E7" s="4">
         <v>2</v>
       </c>
-      <c r="F7" s="17"/>
+      <c r="F7" s="11" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="6">
+      <c r="A8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4">
         <f>ROW()-ROW('Product Backlog'!$B$3)</f>
         <v>5</v>
       </c>
@@ -1147,18 +1175,17 @@
       <c r="E8" s="4">
         <v>3</v>
       </c>
-      <c r="F8" s="17"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>1</v>
+      <c r="A9" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="B9" s="4">
         <f>ROW()-ROW('Product Backlog'!$B$3)</f>
         <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="4">
         <v>3</v>
@@ -1166,33 +1193,31 @@
       <c r="E9" s="4">
         <v>1</v>
       </c>
-      <c r="F9" s="17" t="s">
-        <v>29</v>
+      <c r="F9" s="11" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="str">
-        <f>IF($G$3="", "[Auswählen]")</f>
-        <v>[Auswählen]</v>
+      <c r="A10" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="B10" s="4">
         <f>ROW()-ROW('Product Backlog'!$B$3)</f>
         <v>7</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="4">
         <v>3</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" s="17"/>
+      <c r="E10" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>1</v>
+      <c r="A11" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="B11" s="4">
         <f>ROW()-ROW('Product Backlog'!$B$3)</f>
@@ -1204,14 +1229,13 @@
       <c r="D11" s="4">
         <v>3</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="17"/>
+      <c r="E11" s="4">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>1</v>
+      <c r="A12" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="B12" s="4">
         <f>ROW()-ROW('Product Backlog'!$B$3)</f>
@@ -1223,57 +1247,52 @@
       <c r="D12" s="4">
         <v>3</v>
       </c>
-      <c r="E12" s="4" t="str">
-        <f t="shared" ref="E12:E13" si="0">IF($G$3="", "[Auswählen]")</f>
-        <v>[Auswählen]</v>
-      </c>
-      <c r="F12" s="17"/>
+      <c r="E12" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>1</v>
+      <c r="A13" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="B13" s="4">
         <f>ROW()-ROW('Product Backlog'!$B$3)</f>
         <v>10</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="4">
+        <v>3</v>
+      </c>
+      <c r="E13" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="4">
+        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <v>11</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="D13" s="4">
-        <v>3</v>
-      </c>
-      <c r="E13" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>[Auswählen]</v>
-      </c>
-      <c r="F13" s="17"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="str">
-        <f>IF($G$3="", "[Auswählen]")</f>
-        <v>[Auswählen]</v>
-      </c>
-      <c r="B14" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
-        <v>11</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="D14" s="4">
         <v>5</v>
       </c>
-      <c r="E14" s="6">
-        <v>2</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>32</v>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>1</v>
+      <c r="A15" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="B15" s="4">
         <f>ROW()-ROW('Product Backlog'!$B$3)</f>
@@ -1285,30 +1304,210 @@
       <c r="D15" s="4">
         <v>4</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="4">
         <v>1</v>
       </c>
-      <c r="F15" s="17"/>
+      <c r="F15" s="11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="str">
-        <f>IF($G$3="", "[Auswählen]")</f>
-        <v>[Auswählen]</v>
+      <c r="A16" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B16" s="4">
         <f>ROW()-ROW('Product Backlog'!$B$3)</f>
         <v>13</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="D16" s="4">
         <v>3</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="1">
         <v>4</v>
       </c>
-      <c r="F16" s="17"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="4">
+        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <v>14</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="4">
+        <v>4</v>
+      </c>
+      <c r="E17" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="4">
+        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <v>15</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="4">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="4">
+        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <v>16</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="4">
+        <v>3</v>
+      </c>
+      <c r="E19" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="4">
+        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <v>17</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="4">
+        <v>3</v>
+      </c>
+      <c r="E20" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="4">
+        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <v>18</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="4">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="4">
+        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <v>19</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="4">
+        <v>3</v>
+      </c>
+      <c r="E22" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="4">
+        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <v>20</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="4">
+        <v>3</v>
+      </c>
+      <c r="E23" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="4">
+        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <v>21</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="4">
+        <v>3</v>
+      </c>
+      <c r="E24" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="4">
+        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <v>22</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="4">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="4">
+        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <v>23</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="4">
+        <v>3</v>
+      </c>
+      <c r="E26" s="1">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>

<commit_message>
02_Product_Backlog.xlsx: Aktualisiert, aber noch nicht auf Stand!
</commit_message>
<xml_diff>
--- a/1. Projektplanung/02_Product_Backlog.xlsx
+++ b/1. Projektplanung/02_Product_Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thude0-my.sharepoint.com/personal/jecklu01_hs-ulm_de/Documents/5. Semester/Software Projekt/RaytRazor/1. Projektplanung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="699" documentId="11_AD4DB114E441178AC67DF4622615E776693EDF11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F679B1E5-F3B9-4A40-9364-7E4AA34F1FB5}"/>
+  <xr:revisionPtr revIDLastSave="704" documentId="11_AD4DB114E441178AC67DF4622615E776693EDF11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B645D76-4B7E-46D3-BB5F-D445F0CCFD96}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -159,9 +159,6 @@
     <t>Bild Speicherbar machen.</t>
   </si>
   <si>
-    <t>Kamera muss frei bewegbar.</t>
-  </si>
-  <si>
     <t>Raybounds/Reflektionsanzahl definieren.</t>
   </si>
   <si>
@@ -196,6 +193,9 @@
   </si>
   <si>
     <t>Zuständig: Chriss</t>
+  </si>
+  <si>
+    <t>Kamera muss frei bewegbar sein.</t>
   </si>
 </sst>
 </file>
@@ -383,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -433,26 +433,11 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="15">
     <dxf>
       <fill>
         <patternFill>
@@ -485,139 +470,6 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FF7E11AF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkDown">
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -918,28 +770,24 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{637C7F0C-036B-4704-9330-87E77AC2CA73}" name="Tabelle5" displayName="Tabelle5" ref="A3:F32" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{637C7F0C-036B-4704-9330-87E77AC2CA73}" name="Tabelle5" displayName="Tabelle5" ref="A3:F32" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11">
   <autoFilter ref="A3:F32" xr:uid="{637C7F0C-036B-4704-9330-87E77AC2CA73}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{201166DE-250E-4841-A2FB-745D597FF3E9}" name="Status" dataDxfId="29">
+    <tableColumn id="1" xr3:uid="{201166DE-250E-4841-A2FB-745D597FF3E9}" name="Status" dataDxfId="10">
       <calculatedColumnFormula>IF($G$3="", "[Auswählen]")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{A81DA036-E59B-45ED-99C0-7DA578D2F41E}" name="ID" dataDxfId="28">
+    <tableColumn id="2" xr3:uid="{A81DA036-E59B-45ED-99C0-7DA578D2F41E}" name="ID" dataDxfId="9">
       <calculatedColumnFormula>ROW()-ROW('Product Backlog'!$B$3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{67C87643-0AEC-4F3F-93A3-8AEBECB97CD3}" name="Beschreibung" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{39A480AF-C7AB-4A2D-A3A9-017A9988CD1E}" name="Priorität" dataDxfId="26">
+    <tableColumn id="3" xr3:uid="{67C87643-0AEC-4F3F-93A3-8AEBECB97CD3}" name="Beschreibung" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{39A480AF-C7AB-4A2D-A3A9-017A9988CD1E}" name="Priorität" dataDxfId="7">
       <calculatedColumnFormula>IF($G$3="", "[Auswählen]")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F7F4B23B-3880-466E-A27E-72BD382F2D29}" name="Aufwand" dataDxfId="25">
+    <tableColumn id="5" xr3:uid="{F7F4B23B-3880-466E-A27E-72BD382F2D29}" name="Aufwand" dataDxfId="6">
       <calculatedColumnFormula>IF($G$3="", "[Auswählen]")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9BFAA39F-E911-47E7-A57A-71690B5E810B}" name="Bemerkung" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{9BFAA39F-E911-47E7-A57A-71690B5E810B}" name="Bemerkung" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1223,8 +1071,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A5" zoomScale="175" zoomScaleNormal="205" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A20" zoomScale="175" zoomScaleNormal="205" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1436,7 +1284,7 @@
         <v>4</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1523,7 +1371,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D16" s="4">
         <v>4</v>
@@ -1534,14 +1382,14 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B17" s="4">
         <f>ROW()-ROW('Product Backlog'!$B$3)</f>
         <v>14</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" s="4">
         <v>3</v>
@@ -1559,7 +1407,7 @@
         <v>15</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D18" s="4">
         <v>4</v>
@@ -1577,7 +1425,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D19" s="4">
         <v>4</v>
@@ -1595,7 +1443,7 @@
         <v>17</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20" s="4">
         <v>5</v>
@@ -1604,12 +1452,12 @@
         <v>2</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B21" s="4">
         <f>ROW()-ROW('Product Backlog'!$B$3)</f>
@@ -1663,14 +1511,14 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B24" s="4">
         <f>ROW()-ROW('Product Backlog'!$B$3)</f>
         <v>21</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D24" s="4">
         <v>4</v>
@@ -1760,7 +1608,7 @@
         <v>26</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D29" s="4">
         <v>3</v>
@@ -1778,7 +1626,7 @@
         <v>27</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D30" s="4">
         <v>3</v>
@@ -1788,43 +1636,42 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B31" s="18">
+      <c r="A31" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="4">
         <f>ROW()-ROW('Product Backlog'!$B$3)</f>
         <v>28</v>
       </c>
-      <c r="C31" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="18">
-        <v>2</v>
-      </c>
-      <c r="E31" s="20">
+      <c r="C31" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="4">
+        <v>2</v>
+      </c>
+      <c r="E31" s="1">
         <v>4</v>
       </c>
-      <c r="F31" s="21"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B32" s="18">
+      <c r="A32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="4">
         <f>ROW()-ROW('Product Backlog'!$B$3)</f>
         <v>29</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="C32" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="4">
+        <v>5</v>
+      </c>
+      <c r="E32" s="1">
+        <v>2</v>
+      </c>
+      <c r="F32" s="11" t="s">
         <v>50</v>
-      </c>
-      <c r="D32" s="18">
-        <v>5</v>
-      </c>
-      <c r="E32" s="20">
-        <v>2</v>
-      </c>
-      <c r="F32" s="21" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
02_Product_Backlog.xlsx: Product-Backlog vollständig nachgetragen.
</commit_message>
<xml_diff>
--- a/1. Projektplanung/02_Product_Backlog.xlsx
+++ b/1. Projektplanung/02_Product_Backlog.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thude0-my.sharepoint.com/personal/jecklu01_hs-ulm_de/Documents/5. Semester/Software Projekt/RaytRazor/1. Projektplanung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="704" documentId="11_AD4DB114E441178AC67DF4622615E776693EDF11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B645D76-4B7E-46D3-BB5F-D445F0CCFD96}"/>
+  <xr:revisionPtr revIDLastSave="1100" documentId="11_AD4DB114E441178AC67DF4622615E776693EDF11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FF1A03A-DCE0-4BBE-B600-E7716E76B1D5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="Product-Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Prüfwerte" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="88">
   <si>
     <t>ID</t>
   </si>
@@ -78,12 +78,6 @@
     <t>Product Backlog</t>
   </si>
   <si>
-    <t>Version:</t>
-  </si>
-  <si>
-    <t>1.0.0.0</t>
-  </si>
-  <si>
     <t>Project:</t>
   </si>
   <si>
@@ -123,9 +117,6 @@
     <t>Im Projekt verwendete Raytracing Art wählen.</t>
   </si>
   <si>
-    <t>Gewählt: Diffuses Raytracing</t>
-  </si>
-  <si>
     <t>Visions-Präsentation vorbereiten.</t>
   </si>
   <si>
@@ -147,30 +138,12 @@
     <t>Lichtquellen als 3D Objekt deklarieren.</t>
   </si>
   <si>
-    <t>Lichtquellen Farbe anpassbar machen.</t>
-  </si>
-  <si>
-    <t>Environment/Skybox aufbauen.</t>
-  </si>
-  <si>
-    <t>Demo Szenen aufbauen.</t>
-  </si>
-  <si>
-    <t>Bild Speicherbar machen.</t>
-  </si>
-  <si>
-    <t>Raybounds/Reflektionsanzahl definieren.</t>
-  </si>
-  <si>
     <t>Benutzeroberfläche des Programms erstellen.</t>
   </si>
   <si>
     <t>3D-Objekt Importer erstellen.</t>
   </si>
   <si>
-    <t>JSON Parser implementieren</t>
-  </si>
-  <si>
     <t>Konfigurations Datei definieren</t>
   </si>
   <si>
@@ -192,17 +165,149 @@
     <t>Termin: 21.11.2024</t>
   </si>
   <si>
-    <t>Zuständig: Chriss</t>
-  </si>
-  <si>
-    <t>Kamera muss frei bewegbar sein.</t>
+    <t>Termin: 05.12.2024</t>
+  </si>
+  <si>
+    <t>Sprint Review #4 abgehalten</t>
+  </si>
+  <si>
+    <t>Termin: 19.12.2024</t>
+  </si>
+  <si>
+    <t>Termin: 09.01.2025</t>
+  </si>
+  <si>
+    <t>Product Release</t>
+  </si>
+  <si>
+    <t>Termin: 23.01.2025</t>
+  </si>
+  <si>
+    <t>Meilenstein Präsentation erstellen</t>
+  </si>
+  <si>
+    <t>Meilenstein + Sprint Review #3 abhalten</t>
+  </si>
+  <si>
+    <t>Meilenstein + Sprint Review #5 abgehalten</t>
+  </si>
+  <si>
+    <t>Product Release Management &amp; Technische Präsentation erstellen</t>
+  </si>
+  <si>
+    <t>Raytracing mittels OpenMP Multi-Threaded machen</t>
+  </si>
+  <si>
+    <t>3D Szenen Export implementieren</t>
+  </si>
+  <si>
+    <t>3D-Preview übergabe an Raytracer implementieren</t>
+  </si>
+  <si>
+    <t>Szenen-Manager implementieren</t>
+  </si>
+  <si>
+    <t>Error-Handling im Projekt durch logging verbessern</t>
+  </si>
+  <si>
+    <t>3D-Preview soll mehrere Objekte darstellen können</t>
+  </si>
+  <si>
+    <t>3D-Preview soll Lichtquellen darstellen können</t>
+  </si>
+  <si>
+    <t>3D-Preview soll Objekte aus einer 3D-Szenen JSON anzeigen können</t>
+  </si>
+  <si>
+    <t>JSON Szenen-Import Segmentation Errors beheben</t>
+  </si>
+  <si>
+    <t>Raytracing Bild-Export implementieren</t>
+  </si>
+  <si>
+    <t>JSON Parser Struktur implementieren</t>
+  </si>
+  <si>
+    <t>GitHub Wiki-Page aufbauen</t>
+  </si>
+  <si>
+    <t>3D-Preview Objekte müssen richtig dargestellt werden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raytracer Optimierungen implementieren </t>
+  </si>
+  <si>
+    <t>Szenen-Import soll Szenenauswahl über den Explorer ermöglichen</t>
+  </si>
+  <si>
+    <t>Funktionalität der Top-Bar Buttons implementieren</t>
+  </si>
+  <si>
+    <t>Funktionalität des Component-Trees</t>
+  </si>
+  <si>
+    <t>Schöne Darstellung des Component-Trees</t>
+  </si>
+  <si>
+    <t>Funktionalität der Component Attributes</t>
+  </si>
+  <si>
+    <t>Schöne Darstellung der Component Attributes</t>
+  </si>
+  <si>
+    <t>Raytracing (SDL) in NanoGUI Fenster mit einbinden</t>
+  </si>
+  <si>
+    <t>Dynamische Größenanpassbarkeit des NanoGUI Fensters</t>
+  </si>
+  <si>
+    <t>UI-Darstellung überarbeiten und verschönern</t>
+  </si>
+  <si>
+    <t>Testing und Bug-Fixes</t>
+  </si>
+  <si>
+    <t>Projektziele definieren</t>
+  </si>
+  <si>
+    <t>Benötigte externe Bibliotheken ins Projekt einfügen</t>
+  </si>
+  <si>
+    <t>CMakesList.txt entsprechend anpassen</t>
+  </si>
+  <si>
+    <t>GitHub Actions code-scan Workflow implementieren</t>
+  </si>
+  <si>
+    <t>GitHub Actions build &amp; deploy Workflow implementieren</t>
+  </si>
+  <si>
+    <t>Version des Programms über build &amp; deploy Workflow vergeben</t>
+  </si>
+  <si>
+    <t>Benötigte VERSION.DAT erstellt</t>
+  </si>
+  <si>
+    <t>Grobe Projekt Klassen-Struktur implementieren</t>
+  </si>
+  <si>
+    <t>Component-Klassen implementieren</t>
+  </si>
+  <si>
+    <t>Objekt- und Material Parser implementieren</t>
+  </si>
+  <si>
+    <t>Raytracing mit SDL2 anstatt NanoGUI (OpenGL) implementieren</t>
+  </si>
+  <si>
+    <t>Präsentierbare Demo für Meilenstein-Präsentation fertigstellen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,14 +319,6 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -257,7 +354,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -379,11 +476,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -412,7 +531,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -421,8 +540,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -430,8 +555,20 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -472,6 +609,83 @@
           <bgColor rgb="FF7E11AF"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <top style="thick">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -673,83 +887,6 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <top style="thick">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thick">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right style="thick">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -770,24 +907,28 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{637C7F0C-036B-4704-9330-87E77AC2CA73}" name="Tabelle5" displayName="Tabelle5" ref="A3:F32" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11">
-  <autoFilter ref="A3:F32" xr:uid="{637C7F0C-036B-4704-9330-87E77AC2CA73}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{637C7F0C-036B-4704-9330-87E77AC2CA73}" name="Tabelle5" displayName="Tabelle5" ref="A3:F66" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6">
+  <autoFilter ref="A3:F66" xr:uid="{637C7F0C-036B-4704-9330-87E77AC2CA73}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{201166DE-250E-4841-A2FB-745D597FF3E9}" name="Status" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{201166DE-250E-4841-A2FB-745D597FF3E9}" name="Status" dataDxfId="14">
       <calculatedColumnFormula>IF($G$3="", "[Auswählen]")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{A81DA036-E59B-45ED-99C0-7DA578D2F41E}" name="ID" dataDxfId="9">
-      <calculatedColumnFormula>ROW()-ROW('Product Backlog'!$B$3)</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{A81DA036-E59B-45ED-99C0-7DA578D2F41E}" name="ID" dataDxfId="13">
+      <calculatedColumnFormula>ROW()-ROW('Product-Backlog'!$B$3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{67C87643-0AEC-4F3F-93A3-8AEBECB97CD3}" name="Beschreibung" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{39A480AF-C7AB-4A2D-A3A9-017A9988CD1E}" name="Priorität" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{67C87643-0AEC-4F3F-93A3-8AEBECB97CD3}" name="Beschreibung" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{39A480AF-C7AB-4A2D-A3A9-017A9988CD1E}" name="Priorität" dataDxfId="11">
       <calculatedColumnFormula>IF($G$3="", "[Auswählen]")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F7F4B23B-3880-466E-A27E-72BD382F2D29}" name="Aufwand" dataDxfId="6">
+    <tableColumn id="5" xr3:uid="{F7F4B23B-3880-466E-A27E-72BD382F2D29}" name="Aufwand" dataDxfId="10">
       <calculatedColumnFormula>IF($G$3="", "[Auswählen]")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9BFAA39F-E911-47E7-A57A-71690B5E810B}" name="Bemerkung" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{9BFAA39F-E911-47E7-A57A-71690B5E810B}" name="Bemerkung" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1069,10 +1210,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A20" zoomScale="175" zoomScaleNormal="205" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A33" zoomScale="160" zoomScaleNormal="205" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,27 +1230,23 @@
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:6" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="16"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
@@ -1136,11 +1273,11 @@
         <v>2</v>
       </c>
       <c r="B4" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" s="4">
         <v>5</v>
@@ -1149,7 +1286,7 @@
         <v>2</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1157,11 +1294,11 @@
         <v>2</v>
       </c>
       <c r="B5" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" s="4">
         <v>5</v>
@@ -1170,7 +1307,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1178,11 +1315,11 @@
         <v>2</v>
       </c>
       <c r="B6" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" s="4">
         <v>3</v>
@@ -1196,11 +1333,11 @@
         <v>2</v>
       </c>
       <c r="B7" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>4</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D7" s="4">
         <v>3</v>
@@ -1214,11 +1351,11 @@
         <v>2</v>
       </c>
       <c r="B8" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>5</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" s="4">
         <v>4</v>
@@ -1232,11 +1369,11 @@
         <v>2</v>
       </c>
       <c r="B9" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D9" s="4">
         <v>3</v>
@@ -1244,20 +1381,17 @@
       <c r="E9" s="4">
         <v>1</v>
       </c>
-      <c r="F9" s="11" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>7</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" s="4">
         <v>3</v>
@@ -1271,20 +1405,17 @@
         <v>4</v>
       </c>
       <c r="B11" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>8</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D11" s="4">
         <v>3</v>
       </c>
       <c r="E11" s="4">
         <v>4</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1292,11 +1423,11 @@
         <v>2</v>
       </c>
       <c r="B12" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>9</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D12" s="4">
         <v>3</v>
@@ -1310,11 +1441,11 @@
         <v>2</v>
       </c>
       <c r="B13" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>10</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D13" s="4">
         <v>3</v>
@@ -1328,11 +1459,11 @@
         <v>2</v>
       </c>
       <c r="B14" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>11</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D14" s="4">
         <v>5</v>
@@ -1341,7 +1472,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1349,11 +1480,11 @@
         <v>2</v>
       </c>
       <c r="B15" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>12</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D15" s="4">
         <v>4</v>
@@ -1367,11 +1498,11 @@
         <v>2</v>
       </c>
       <c r="B16" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>13</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D16" s="4">
         <v>4</v>
@@ -1385,11 +1516,11 @@
         <v>2</v>
       </c>
       <c r="B17" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>14</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D17" s="4">
         <v>3</v>
@@ -1403,11 +1534,11 @@
         <v>2</v>
       </c>
       <c r="B18" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>15</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D18" s="4">
         <v>4</v>
@@ -1418,14 +1549,14 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B19" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>16</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D19" s="4">
         <v>4</v>
@@ -1439,11 +1570,11 @@
         <v>2</v>
       </c>
       <c r="B20" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>17</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D20" s="4">
         <v>5</v>
@@ -1452,7 +1583,7 @@
         <v>2</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1460,11 +1591,11 @@
         <v>2</v>
       </c>
       <c r="B21" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>18</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D21" s="4">
         <v>3</v>
@@ -1475,14 +1606,14 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B22" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>19</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D22" s="4">
         <v>3</v>
@@ -1493,14 +1624,14 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B23" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>20</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D23" s="4">
         <v>3</v>
@@ -1514,11 +1645,11 @@
         <v>2</v>
       </c>
       <c r="B24" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>21</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="D24" s="4">
         <v>4</v>
@@ -1529,149 +1660,811 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B25" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>22</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D25" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E25" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B26" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>23</v>
       </c>
       <c r="C26" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="4">
+        <v>5</v>
+      </c>
+      <c r="E26" s="1">
+        <v>2</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>24</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="19">
+        <v>4</v>
+      </c>
+      <c r="E27" s="21">
+        <v>4</v>
+      </c>
+      <c r="F27" s="22"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>25</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="19">
+        <v>4</v>
+      </c>
+      <c r="E28" s="21">
+        <v>4</v>
+      </c>
+      <c r="F28" s="22"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>26</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="19">
+        <v>4</v>
+      </c>
+      <c r="E29" s="21">
+        <v>4</v>
+      </c>
+      <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>27</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="19">
+        <v>4</v>
+      </c>
+      <c r="E30" s="21">
+        <v>4</v>
+      </c>
+      <c r="F30" s="22"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>28</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="19">
+        <v>4</v>
+      </c>
+      <c r="E31" s="21">
+        <v>4</v>
+      </c>
+      <c r="F31" s="22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>29</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="19">
+        <v>4</v>
+      </c>
+      <c r="E32" s="21">
+        <v>3</v>
+      </c>
+      <c r="F32" s="22"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>30</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" s="19">
+        <v>4</v>
+      </c>
+      <c r="E33" s="21">
+        <v>3</v>
+      </c>
+      <c r="F33" s="22"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>31</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D34" s="19">
+        <v>4</v>
+      </c>
+      <c r="E34" s="21">
+        <v>4</v>
+      </c>
+      <c r="F34" s="22"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>32</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="19">
+        <v>4</v>
+      </c>
+      <c r="E35" s="21">
+        <v>4</v>
+      </c>
+      <c r="F35" s="22"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>33</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="19">
+        <v>4</v>
+      </c>
+      <c r="E36" s="21">
+        <v>4</v>
+      </c>
+      <c r="F36" s="22"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>34</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="19">
+        <v>5</v>
+      </c>
+      <c r="E37" s="21">
+        <v>3</v>
+      </c>
+      <c r="F37" s="22"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>35</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="19">
+        <v>5</v>
+      </c>
+      <c r="E38" s="21">
+        <v>2</v>
+      </c>
+      <c r="F38" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>36</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" s="19">
+        <v>4</v>
+      </c>
+      <c r="E39" s="21">
+        <v>3</v>
+      </c>
+      <c r="F39" s="22"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>37</v>
       </c>
-      <c r="D26" s="4">
-        <v>3</v>
-      </c>
-      <c r="E26" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
-        <v>24</v>
-      </c>
-      <c r="C27" s="5" t="s">
+      <c r="C40" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" s="19">
+        <v>4</v>
+      </c>
+      <c r="E40" s="21">
+        <v>2</v>
+      </c>
+      <c r="F40" s="22"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>38</v>
       </c>
-      <c r="D27" s="4">
-        <v>3</v>
-      </c>
-      <c r="E27" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
-        <v>25</v>
-      </c>
-      <c r="C28" s="5" t="s">
+      <c r="C41" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41" s="19">
+        <v>5</v>
+      </c>
+      <c r="E41" s="21">
+        <v>2</v>
+      </c>
+      <c r="F41" s="22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>39</v>
       </c>
-      <c r="D28" s="4">
-        <v>3</v>
-      </c>
-      <c r="E28" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
-        <v>26</v>
-      </c>
-      <c r="C29" s="5" t="s">
+      <c r="C42" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" s="19">
+        <v>3</v>
+      </c>
+      <c r="E42" s="21">
+        <v>3</v>
+      </c>
+      <c r="F42" s="22"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>40</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" s="19">
+        <v>4</v>
+      </c>
+      <c r="E43" s="21">
+        <v>3</v>
+      </c>
+      <c r="F43" s="22"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>41</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" s="19">
+        <v>4</v>
+      </c>
+      <c r="E44" s="21">
+        <v>3</v>
+      </c>
+      <c r="F44" s="22"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>42</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="19">
+        <v>3</v>
+      </c>
+      <c r="E45" s="21">
+        <v>2</v>
+      </c>
+      <c r="F45" s="22"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>43</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D46" s="19">
+        <v>4</v>
+      </c>
+      <c r="E46" s="21">
+        <v>4</v>
+      </c>
+      <c r="F46" s="22"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>44</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D47" s="19">
+        <v>4</v>
+      </c>
+      <c r="E47" s="21">
+        <v>3</v>
+      </c>
+      <c r="F47" s="22"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>45</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D48" s="19">
+        <v>4</v>
+      </c>
+      <c r="E48" s="21">
+        <v>4</v>
+      </c>
+      <c r="F48" s="22"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>46</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D49" s="19">
+        <v>4</v>
+      </c>
+      <c r="E49" s="21">
+        <v>3</v>
+      </c>
+      <c r="F49" s="22"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>47</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D50" s="19">
+        <v>5</v>
+      </c>
+      <c r="E50" s="21">
+        <v>2</v>
+      </c>
+      <c r="F50" s="22"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>48</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D51" s="19">
+        <v>2</v>
+      </c>
+      <c r="E51" s="21">
+        <v>3</v>
+      </c>
+      <c r="F51" s="22"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>49</v>
+      </c>
+      <c r="C52" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D52" s="19">
+        <v>3</v>
+      </c>
+      <c r="E52" s="21">
+        <v>4</v>
+      </c>
+      <c r="F52" s="22"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>50</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D53" s="19">
+        <v>3</v>
+      </c>
+      <c r="E53" s="21">
+        <v>4</v>
+      </c>
+      <c r="F53" s="22"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>51</v>
+      </c>
+      <c r="C54" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D54" s="19">
+        <v>5</v>
+      </c>
+      <c r="E54" s="21">
+        <v>2</v>
+      </c>
+      <c r="F54" s="22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
         <v>52</v>
       </c>
-      <c r="D29" s="4">
-        <v>3</v>
-      </c>
-      <c r="E29" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
-        <v>27</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="4">
-        <v>3</v>
-      </c>
-      <c r="E30" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
-        <v>28</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" s="4">
-        <v>2</v>
-      </c>
-      <c r="E31" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B32" s="4">
-        <f>ROW()-ROW('Product Backlog'!$B$3)</f>
-        <v>29</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D32" s="4">
+      <c r="C55" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D55" s="19">
         <v>5</v>
       </c>
-      <c r="E32" s="1">
-        <v>2</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>50</v>
+      <c r="E55" s="21">
+        <v>3</v>
+      </c>
+      <c r="F55" s="22"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>53</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D56" s="19">
+        <v>4</v>
+      </c>
+      <c r="E56" s="21">
+        <v>4</v>
+      </c>
+      <c r="F56" s="22"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>54</v>
+      </c>
+      <c r="C57" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D57" s="19">
+        <v>4</v>
+      </c>
+      <c r="E57" s="21">
+        <v>3</v>
+      </c>
+      <c r="F57" s="22"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B58" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>55</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D58" s="19">
+        <v>4</v>
+      </c>
+      <c r="E58" s="21">
+        <v>2</v>
+      </c>
+      <c r="F58" s="22"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>56</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D59" s="19">
+        <v>4</v>
+      </c>
+      <c r="E59" s="21">
+        <v>3</v>
+      </c>
+      <c r="F59" s="22"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>57</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D60" s="19">
+        <v>4</v>
+      </c>
+      <c r="E60" s="21">
+        <v>3</v>
+      </c>
+      <c r="F60" s="22"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>58</v>
+      </c>
+      <c r="C61" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D61" s="19">
+        <v>4</v>
+      </c>
+      <c r="E61" s="21">
+        <v>3</v>
+      </c>
+      <c r="F61" s="22"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B62" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>59</v>
+      </c>
+      <c r="C62" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D62" s="19">
+        <v>4</v>
+      </c>
+      <c r="E62" s="21">
+        <v>3</v>
+      </c>
+      <c r="F62" s="22"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>60</v>
+      </c>
+      <c r="C63" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D63" s="19">
+        <v>4</v>
+      </c>
+      <c r="E63" s="21">
+        <v>3</v>
+      </c>
+      <c r="F63" s="22"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B64" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>61</v>
+      </c>
+      <c r="C64" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D64" s="19">
+        <v>4</v>
+      </c>
+      <c r="E64" s="21">
+        <v>3</v>
+      </c>
+      <c r="F64" s="22"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>62</v>
+      </c>
+      <c r="C65" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D65" s="19">
+        <v>5</v>
+      </c>
+      <c r="E65" s="21">
+        <v>3</v>
+      </c>
+      <c r="F65" s="22"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" s="19">
+        <f>ROW()-ROW('Product-Backlog'!$B$3)</f>
+        <v>63</v>
+      </c>
+      <c r="C66" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D66" s="19">
+        <v>5</v>
+      </c>
+      <c r="E66" s="21">
+        <v>3</v>
+      </c>
+      <c r="F66" s="22" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>